<commit_message>
Add AutoCopyrightCoveredResourcedExcelBuilder to add column resource page Update CoverSheet.xlsx template to be more clean and compatible
</commit_message>
<xml_diff>
--- a/Medidata.Rave.Tsdv.Loader/Resources/CoverSheet.xlsx
+++ b/Medidata.Rave.Tsdv.Loader/Resources/CoverSheet.xlsx
@@ -9,12 +9,6 @@
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 

</xml_diff>

<commit_message>
Update column source logic
Add AutoCopyrightCoveredResourcedExcelBuilder to add column resource page
Update CoverSheet.xlsx template to be more clean and compatible
</commit_message>
<xml_diff>
--- a/Medidata.Rave.Tsdv.Loader/Resources/CoverSheet.xlsx
+++ b/Medidata.Rave.Tsdv.Loader/Resources/CoverSheet.xlsx
@@ -9,12 +9,6 @@
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 

</xml_diff>